<commit_message>
Add tag_master.xlsx with 39 clinics
</commit_message>
<xml_diff>
--- a/model_data/tag_master.xlsx
+++ b/model_data/tag_master.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,72 +448,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>areas</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>診療</t>
+          <t>さくら歯科</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>areas</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>予防</t>
+          <t>たんぽぽ歯科</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>areas</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>矯正</t>
+          <t>ありす歯科</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>areas</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>インプラント</t>
+          <t>春日井きらり歯科</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>areas</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>審美</t>
+          <t>松戸ありす歯科</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>areas</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>訪問診療</t>
+          <t>池下さくら歯科</t>
         </is>
       </c>
     </row>
@@ -525,113 +525,497 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>さくら歯科 本院</t>
+          <t>日進赤池たんぽぽ歯科</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>positions</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>歯科医師</t>
+          <t>春日井アップル歯科</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>positions</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>歯科衛生士</t>
+          <t>緑区さくら医院・歯科</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>positions</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>歯科助手</t>
+          <t>緑区さくら医院・医科</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>positions</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>受付</t>
+          <t>緑区さくら医院・健診</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>positions</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>事務</t>
+          <t>金沢さくら医院・健診</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>positions</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>マネージャー</t>
+          <t>金沢さくら医院・婦人科</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>ハピネス歯科</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>clinics</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>leave</t>
+          <t>流山ハピネス歯科</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>イーアス春日井</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>名駅さくら医院・名古屋歯科・歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>名駅さくら医院・名古屋歯科・内科</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>名駅さくら医院・名古屋歯科・皮膚科</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>きらり大森歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>クローバー歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>流山ありす歯科・矯正歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>長久手さくら歯科・矯正歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ヒロデンタル</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>町屋さくら歯科・矯正歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>金沢さくら医院 歯科</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>きた矯正歯科クリニック</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>デンタルオフィス増田</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>祥南歯科・矯正歯科医院</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>三田矯正歯科医院</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>グランド歯科医院</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>訪問部（春日井事務所）</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>訪問部（杁中事務所）</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>春日井事務局</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>名古屋駅JPタワー事務所</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>いりなか事務所</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>池下事務所</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>流山事務所</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>clinics</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>浄心事務所</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>positions</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>歯科医師</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>positions</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>歯科衛生士</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>positions</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>歯科助手</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>positions</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>受付</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>positions</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>事務</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>positions</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>マネージャー</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
           <t>status</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>leave</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>retired</t>
         </is>

</xml_diff>